<commit_message>
Correction des valeurs de courbe de charge pour la production solaire d'un facteur de 1000
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/Courbe de charge Solaire.xlsx
+++ b/Projet-Groupe1-DKM/data/Courbe de charge Solaire.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yomal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83130049-F022-4533-9633-528D16E33F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51CF50B-49DC-4859-BD48-0322C084EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5856" yWindow="2772" windowWidth="17280" windowHeight="8880" xr2:uid="{8F64D4BE-3042-492D-916E-AB5D810A7B0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F64D4BE-3042-492D-916E-AB5D810A7B0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -88,15 +88,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -186,7 +185,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="fr-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -325,73 +324,73 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.450999683732439</c:v>
+                  <c:v>2.4509996837324389E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8563418808264371</c:v>
+                  <c:v>4.8563418808264371E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1712196172323459</c:v>
+                  <c:v>7.1712196172323463E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3525111006378019</c:v>
+                  <c:v>9.352511100637801E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.35958299786895</c:v>
+                  <c:v>1.1359582997868949E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.155047357006231</c:v>
+                  <c:v>1.315504735700623E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.705458074187961</c:v>
+                  <c:v>1.4705458074187961E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.98193393124275</c:v>
+                  <c:v>1.598193393124275E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.960696598138771</c:v>
+                  <c:v>1.6960696598138772E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.623513578281809</c:v>
+                  <c:v>1.7623513578281808E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.958037845429711</c:v>
+                  <c:v>1.7958037845429712E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.9580378454297</c:v>
+                  <c:v>1.7958037845429702E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.62351357828182</c:v>
+                  <c:v>1.7623513578281819E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.960696598138771</c:v>
+                  <c:v>1.6960696598138772E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.981933931242761</c:v>
+                  <c:v>1.598193393124276E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.705458074187961</c:v>
+                  <c:v>1.4705458074187961E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.155047357006239</c:v>
+                  <c:v>1.315504735700624E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.35958299786895</c:v>
+                  <c:v>1.1359582997868949E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.352511100637809</c:v>
+                  <c:v>9.3525111006378097E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.171219617232353</c:v>
+                  <c:v>7.1712196172323533E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.8563418808264371</c:v>
+                  <c:v>4.8563418808264371E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.4509996837324399</c:v>
+                  <c:v>2.4509996837324397E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2043642384652358E-15</c:v>
+                  <c:v>2.2043642384652359E-18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,73 +531,73 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8382497627993291</c:v>
+                  <c:v>1.838249762799329E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6422564106198281</c:v>
+                  <c:v>3.642256410619828E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3784147129242594</c:v>
+                  <c:v>5.3784147129242593E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0143833254783514</c:v>
+                  <c:v>7.0143833254783516E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.519687248401711</c:v>
+                  <c:v>8.5196872484017104E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.866285517754676</c:v>
+                  <c:v>9.8662855177546766E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.029093555640969</c:v>
+                  <c:v>1.1029093555640969E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.986450448432061</c:v>
+                  <c:v>1.1986450448432062E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.720522448604081</c:v>
+                  <c:v>1.2720522448604081E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.21763518371136</c:v>
+                  <c:v>1.3217635183711361E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.468528384072281</c:v>
+                  <c:v>1.3468528384072281E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.468528384072281</c:v>
+                  <c:v>1.3468528384072281E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.21763518371136</c:v>
+                  <c:v>1.3217635183711361E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.720522448604081</c:v>
+                  <c:v>1.2720522448604081E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.986450448432061</c:v>
+                  <c:v>1.1986450448432062E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.029093555640969</c:v>
+                  <c:v>1.1029093555640969E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.8662855177546795</c:v>
+                  <c:v>9.8662855177546801E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5196872484017145</c:v>
+                  <c:v>8.5196872484017139E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.0143833254783559</c:v>
+                  <c:v>7.014383325478356E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.3784147129242648</c:v>
+                  <c:v>5.3784147129242645E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.6422564106198281</c:v>
+                  <c:v>3.642256410619828E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.8382497627993299</c:v>
+                  <c:v>1.8382497627993299E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.6532731788489271E-15</c:v>
+                  <c:v>1.653273178848927E-18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1857,313 +1856,313 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>60437</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.450999683732439</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.8382497627993291</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="B3">
+        <v>2.4509996837324389E-3</v>
+      </c>
+      <c r="C3">
+        <v>1.838249762799329E-3</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B4" s="1">
-        <v>4.8563418808264371</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.6422564106198281</v>
-      </c>
-      <c r="D4" s="4"/>
+      <c r="B4">
+        <v>4.8563418808264371E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.642256410619828E-3</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>0.125</v>
       </c>
-      <c r="B5" s="1">
-        <v>7.1712196172323459</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.3784147129242594</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="B5">
+        <v>7.1712196172323463E-3</v>
+      </c>
+      <c r="C5">
+        <v>5.3784147129242593E-3</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B6" s="1">
-        <v>9.3525111006378019</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7.0143833254783514</v>
-      </c>
-      <c r="D6" s="4"/>
+      <c r="B6">
+        <v>9.352511100637801E-3</v>
+      </c>
+      <c r="C6">
+        <v>7.0143833254783516E-3</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B7" s="1">
-        <v>11.35958299786895</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8.519687248401711</v>
-      </c>
-      <c r="D7" s="4"/>
+      <c r="B7">
+        <v>1.1359582997868949E-2</v>
+      </c>
+      <c r="C7">
+        <v>8.5196872484017104E-3</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0.25</v>
       </c>
-      <c r="B8" s="1">
-        <v>13.155047357006231</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9.866285517754676</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="B8">
+        <v>1.315504735700623E-2</v>
+      </c>
+      <c r="C8">
+        <v>9.8662855177546766E-3</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B9" s="1">
-        <v>14.705458074187961</v>
-      </c>
-      <c r="C9" s="1">
-        <v>11.029093555640969</v>
-      </c>
-      <c r="D9" s="4"/>
+      <c r="B9">
+        <v>1.4705458074187961E-2</v>
+      </c>
+      <c r="C9">
+        <v>1.1029093555640969E-2</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B10" s="1">
-        <v>15.98193393124275</v>
-      </c>
-      <c r="C10" s="1">
-        <v>11.986450448432061</v>
-      </c>
-      <c r="D10" s="4"/>
+      <c r="B10">
+        <v>1.598193393124275E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.1986450448432062E-2</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>0.375</v>
       </c>
-      <c r="B11" s="1">
-        <v>16.960696598138771</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12.720522448604081</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="B11">
+        <v>1.6960696598138772E-2</v>
+      </c>
+      <c r="C11">
+        <v>1.2720522448604081E-2</v>
+      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="1">
-        <v>17.623513578281809</v>
-      </c>
-      <c r="C12" s="1">
-        <v>13.21763518371136</v>
-      </c>
-      <c r="D12" s="4"/>
+      <c r="B12">
+        <v>1.7623513578281808E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.3217635183711361E-2</v>
+      </c>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B13" s="1">
-        <v>17.958037845429711</v>
-      </c>
-      <c r="C13" s="1">
-        <v>13.468528384072281</v>
-      </c>
-      <c r="D13" s="4"/>
+      <c r="B13">
+        <v>1.7958037845429712E-2</v>
+      </c>
+      <c r="C13">
+        <v>1.3468528384072281E-2</v>
+      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>0.5</v>
       </c>
-      <c r="B14" s="1">
-        <v>17.9580378454297</v>
-      </c>
-      <c r="C14" s="1">
-        <v>13.468528384072281</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="B14">
+        <v>1.7958037845429702E-2</v>
+      </c>
+      <c r="C14">
+        <v>1.3468528384072281E-2</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="1">
-        <v>17.62351357828182</v>
-      </c>
-      <c r="C15" s="1">
-        <v>13.21763518371136</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="B15">
+        <v>1.7623513578281819E-2</v>
+      </c>
+      <c r="C15">
+        <v>1.3217635183711361E-2</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B16" s="1">
-        <v>16.960696598138771</v>
-      </c>
-      <c r="C16" s="1">
-        <v>12.720522448604081</v>
-      </c>
-      <c r="D16" s="4"/>
+      <c r="B16">
+        <v>1.6960696598138772E-2</v>
+      </c>
+      <c r="C16">
+        <v>1.2720522448604081E-2</v>
+      </c>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>0.625</v>
       </c>
-      <c r="B17" s="1">
-        <v>15.981933931242761</v>
-      </c>
-      <c r="C17" s="1">
-        <v>11.986450448432061</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="B17">
+        <v>1.598193393124276E-2</v>
+      </c>
+      <c r="C17">
+        <v>1.1986450448432062E-2</v>
+      </c>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B18" s="1">
-        <v>14.705458074187961</v>
-      </c>
-      <c r="C18" s="1">
-        <v>11.029093555640969</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="B18">
+        <v>1.4705458074187961E-2</v>
+      </c>
+      <c r="C18">
+        <v>1.1029093555640969E-2</v>
+      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B19" s="1">
-        <v>13.155047357006239</v>
-      </c>
-      <c r="C19" s="1">
-        <v>9.8662855177546795</v>
-      </c>
-      <c r="D19" s="4"/>
+      <c r="B19">
+        <v>1.315504735700624E-2</v>
+      </c>
+      <c r="C19">
+        <v>9.8662855177546801E-3</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>0.75</v>
       </c>
-      <c r="B20" s="1">
-        <v>11.35958299786895</v>
-      </c>
-      <c r="C20" s="1">
-        <v>8.5196872484017145</v>
-      </c>
-      <c r="D20" s="4"/>
+      <c r="B20">
+        <v>1.1359582997868949E-2</v>
+      </c>
+      <c r="C20">
+        <v>8.5196872484017139E-3</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B21" s="1">
-        <v>9.352511100637809</v>
-      </c>
-      <c r="C21" s="1">
-        <v>7.0143833254783559</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="B21">
+        <v>9.3525111006378097E-3</v>
+      </c>
+      <c r="C21">
+        <v>7.014383325478356E-3</v>
+      </c>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>0.83333333333333304</v>
       </c>
-      <c r="B22" s="1">
-        <v>7.171219617232353</v>
-      </c>
-      <c r="C22" s="1">
-        <v>5.3784147129242648</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="B22">
+        <v>7.1712196172323533E-3</v>
+      </c>
+      <c r="C22">
+        <v>5.3784147129242645E-3</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>0.875</v>
       </c>
-      <c r="B23" s="1">
-        <v>4.8563418808264371</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3.6422564106198281</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="B23">
+        <v>4.8563418808264371E-3</v>
+      </c>
+      <c r="C23">
+        <v>3.642256410619828E-3</v>
+      </c>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>0.91666666666666696</v>
       </c>
-      <c r="B24" s="1">
-        <v>2.4509996837324399</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.8382497627993299</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="B24">
+        <v>2.4509996837324397E-3</v>
+      </c>
+      <c r="C24">
+        <v>1.8382497627993299E-3</v>
+      </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>0.95833333333333304</v>
       </c>
-      <c r="B25" s="1">
-        <v>2.2043642384652358E-15</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.6532731788489271E-15</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="B25">
+        <v>2.2043642384652359E-18</v>
+      </c>
+      <c r="C25">
+        <v>1.653273178848927E-18</v>
+      </c>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D26" s="4"/>
+      <c r="D26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>